<commit_message>
tests working on mil
</commit_message>
<xml_diff>
--- a/requirements-shc.xlsx
+++ b/requirements-shc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\smart-testing-genai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D1D85C-1F6D-47FA-B031-E746F90350CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D2C916-2E86-4416-BA57-FE701DB5615B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22920" windowHeight="13800" xr2:uid="{A1A5982F-B6D4-7141-8338-8EF5079164CC}"/>
+    <workbookView xWindow="2175" yWindow="2175" windowWidth="15210" windowHeight="8835" xr2:uid="{A1A5982F-B6D4-7141-8338-8EF5079164CC}"/>
   </bookViews>
   <sheets>
     <sheet name="shc" sheetId="1" r:id="rId1"/>
@@ -563,15 +563,15 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="107.375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.875" style="1"/>
+    <col min="2" max="2" width="24.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="107.38671875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25">
@@ -641,7 +641,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25">
+    <row r="8" spans="1:3" ht="45">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -652,7 +652,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="47.25">
+    <row r="9" spans="1:3" ht="45">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -663,7 +663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="47.25">
+    <row r="10" spans="1:3" ht="45">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -674,7 +674,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="47.25">
+    <row r="11" spans="1:3" ht="45">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>

</xml_diff>